<commit_message>
fix bic and cp
</commit_message>
<xml_diff>
--- a/tests/data/sas_benchmark.xlsx
+++ b/tests/data/sas_benchmark.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kai/GitHub/StepReg/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lij11/Dropbox (UMass Medical School)/Project/UMMS/Github/JunhuiLi1017/StepReg/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06ED3964-F7B1-5B41-8CDB-617CB849023B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4896737A-398C-0347-B9E0-9D9C30F42B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="5240" windowWidth="23720" windowHeight="13900" xr2:uid="{29101AD1-6FAF-C449-8C59-8CA43C027762}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{29101AD1-6FAF-C449-8C59-8CA43C027762}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="36">
   <si>
     <t>test model</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>bidirection</t>
-  </si>
-  <si>
-    <t>NA (can be done by sas though)</t>
   </si>
   <si>
     <t>subset</t>
@@ -538,7 +535,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +617,7 @@
         <v>7</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -811,8 +808,8 @@
       <c r="K9" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>27</v>
+      <c r="L9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -942,7 +939,7 @@
         <v>19</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>26</v>
@@ -951,7 +948,7 @@
         <v>19</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -965,7 +962,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
@@ -974,7 +971,7 @@
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>26</v>
@@ -983,7 +980,7 @@
         <v>6</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -997,7 +994,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
         <v>24</v>
@@ -1006,7 +1003,7 @@
         <v>8</v>
       </c>
       <c r="H16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>26</v>
@@ -1015,7 +1012,7 @@
         <v>8</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1029,7 +1026,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" t="s">
         <v>24</v>
@@ -1038,7 +1035,7 @@
         <v>20</v>
       </c>
       <c r="H17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>26</v>
@@ -1047,7 +1044,7 @@
         <v>20</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1122,28 +1119,28 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1154,33 +1151,33 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" t="s">
         <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
@@ -1189,7 +1186,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
         <v>24</v>
@@ -1198,7 +1195,7 @@
         <v>19</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>26</v>
@@ -1206,7 +1203,7 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -1215,12 +1212,12 @@
         <v>6</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
@@ -1229,12 +1226,12 @@
         <v>8</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -1243,12 +1240,12 @@
         <v>20</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -1262,7 +1259,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
@@ -1276,30 +1273,30 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>